<commit_message>
QA Activity update as on 14.08.2018
</commit_message>
<xml_diff>
--- a/QA-Activities.xlsx
+++ b/QA-Activities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="270718" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,11 @@
     <sheet name="060818" sheetId="13" r:id="rId7"/>
     <sheet name="070818" sheetId="15" r:id="rId8"/>
     <sheet name="080818" sheetId="14" r:id="rId9"/>
-    <sheet name="Today" sheetId="17" r:id="rId10"/>
+    <sheet name="090818" sheetId="17" r:id="rId10"/>
+    <sheet name="100818" sheetId="18" r:id="rId11"/>
+    <sheet name="130818" sheetId="20" r:id="rId12"/>
+    <sheet name="Today" sheetId="21" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'010818'!$C$1:$C$10</definedName>
@@ -25,7 +29,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'060818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'070818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'080818'!$C$1:$C$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Today!$C$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'090818'!$C$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'100818'!$C$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'130818'!$C$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Today!$C$1:$C$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="186">
   <si>
     <t>#</t>
   </si>
@@ -781,6 +788,123 @@
   </si>
   <si>
     <t>Complete Location</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generate Scenario- Collaborated scenario of Data upload and Generate EWB
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Load testing scenarios . </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Send report.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Report in progress
+Demo setup in progress
+Test run in new db -inprogress  
+Test data creation -inprogress</t>
+  </si>
+  <si>
+    <t>Need to analyse details and send report</t>
+  </si>
+  <si>
+    <t>Framework setup in progress</t>
+  </si>
+  <si>
+    <t>Integrating with new framework inprogress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrating with new framework </t>
+  </si>
+  <si>
+    <t>Framework setup</t>
+  </si>
+  <si>
+    <t>LEAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Scenario- Collaborated scenario of Data upload and Generate EWB
+Need to analyse details and send report
+</t>
+  </si>
+  <si>
+    <t>Frame work setup and demo completed
+Feedback After Demo :
+1.Check NIC Status till its get updated.(generate,update vechicle,cancel ewb)
+2.Include screen shots in test output.
+3.Slow down the scenarios for demo.
+4.Need Html report.
+5.Run as zoot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Check NIC Status till its get updated.(generate)
+2.Include screen shots in test output.
+3.Slow down the scenarios for demo.
+4.Need Html report.
+</t>
+  </si>
+  <si>
+    <t>1. Check NIC Status till its get updated.(update vechicle,cancel ewb)
+2. TRA_4 : Transporter can update vehicle</t>
+  </si>
+  <si>
+    <t>Report preparation completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check NIC Status till its get updated.(update vechicle,cancel ewb)
+2. TRA_4 : Transporter can update vehicle </t>
+  </si>
+  <si>
+    <t>1.Check NIC Status till its get updated.(generate)
+2.Include screen shots in test output.
+3.Slow down the scenarios for demo.
+4.Need Html report.</t>
+  </si>
+  <si>
+    <t>TRA_4 : Transporter can update vehicle</t>
+  </si>
+  <si>
+    <t>1.Check NIC Status till its get updated.(generate)-Completed
+2.Include screen shots in test output.-Inprogress
+3.Slow down the scenarios for demo.-Inprogress
+4.Need Html report.-Completed
+5.Run as zoot - Inprogress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Include screen shots in test output.
+3.Slow down the scenarios for demo.
+5.Run as zoot </t>
+  </si>
+  <si>
+    <t>1. Check NIC Status till its get updated.(update vechicle,cancel ewb)-Completed
+2. TRA_4 : Transporter can update vehicle -Inprogress
+Transporter listing issue found in demo2 instance.So created a new user in demo7 and checked whether data is loaded for transporter.</t>
+  </si>
+  <si>
+    <t>Locn Mstr_1 to 5</t>
+  </si>
+  <si>
+    <t>Locn Mstr_6 to 9</t>
   </si>
 </sst>
 </file>
@@ -834,7 +958,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -981,11 +1105,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1097,6 +1239,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1113,6 +1276,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1420,7 +1592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1556,7 +1728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1574,36 +1746,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="35" t="s">
         <v>9</v>
       </c>
@@ -1730,6 +1902,531 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="44.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="7">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:F36">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="44.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="50"/>
+      <c r="H5" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="8">
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:F36">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="44.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="7">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:F35">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1754,36 +2451,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="16" t="s">
         <v>9</v>
       </c>
@@ -2037,36 +2734,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
@@ -2321,36 +3018,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
@@ -2599,36 +3296,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="18" t="s">
         <v>9</v>
       </c>
@@ -2780,36 +3477,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
@@ -2961,36 +3658,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="23" t="s">
         <v>9</v>
       </c>
@@ -3142,36 +3839,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="27" t="s">
         <v>9</v>
       </c>
@@ -3323,36 +4020,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="26" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Testing status as on 16.08.2018
</commit_message>
<xml_diff>
--- a/QA-Activities.xlsx
+++ b/QA-Activities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="270718" sheetId="9" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="090818" sheetId="17" r:id="rId10"/>
     <sheet name="100818" sheetId="18" r:id="rId11"/>
     <sheet name="130818" sheetId="20" r:id="rId12"/>
-    <sheet name="Today" sheetId="21" r:id="rId13"/>
-    <sheet name="Sheet1" sheetId="19" r:id="rId14"/>
+    <sheet name="140818" sheetId="21" r:id="rId13"/>
+    <sheet name="Today" sheetId="22" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'010818'!$C$1:$C$10</definedName>
@@ -32,7 +33,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'090818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'100818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'130818'!$C$1:$C$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Today!$C$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'140818'!$C$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Today!$C$1:$C$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="191">
   <si>
     <t>#</t>
   </si>
@@ -905,6 +907,24 @@
   </si>
   <si>
     <t>Locn Mstr_6 to 9</t>
+  </si>
+  <si>
+    <t>TRA_4 : Transporter can update vehicle - Completed
+TRA_8 : Transporter can update movement - Inprogress</t>
+  </si>
+  <si>
+    <t>2.Include screen shots in test output. -Completed
+3.Slow down the scenarios for demo.-Inprogress
+5.Run as zoot -Completed</t>
+  </si>
+  <si>
+    <t>TRA_8 : Transporter can update movement</t>
+  </si>
+  <si>
+    <t>3.Slow down the scenarios for demo.</t>
+  </si>
+  <si>
+    <t>Gst Mstr_1 to 4</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1260,6 +1280,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1282,9 +1308,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1592,7 +1615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1746,36 +1769,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="35" t="s">
         <v>9</v>
       </c>
@@ -1927,36 +1950,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="36" t="s">
         <v>9</v>
       </c>
@@ -2108,36 +2131,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="37" t="s">
         <v>9</v>
       </c>
@@ -2189,7 +2212,7 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="51" t="s">
         <v>174</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -2215,7 +2238,7 @@
       <c r="F5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="50"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="9" t="s">
         <v>175</v>
       </c>
@@ -2268,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,36 +2309,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2390,10 +2413,10 @@
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="44" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2419,6 +2442,160 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="44.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="7">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:F35">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2451,36 +2628,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="16" t="s">
         <v>9</v>
       </c>
@@ -2734,36 +2911,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
@@ -3018,36 +3195,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
@@ -3296,36 +3473,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>9</v>
       </c>
@@ -3477,36 +3654,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
@@ -3658,36 +3835,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="23" t="s">
         <v>9</v>
       </c>
@@ -3839,36 +4016,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="27" t="s">
         <v>9</v>
       </c>
@@ -4020,36 +4197,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="26" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Offshore Testing status as on 17.08.2018
</commit_message>
<xml_diff>
--- a/QA-Activities.xlsx
+++ b/QA-Activities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="270718" sheetId="9" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="100818" sheetId="18" r:id="rId11"/>
     <sheet name="130818" sheetId="20" r:id="rId12"/>
     <sheet name="140818" sheetId="21" r:id="rId13"/>
-    <sheet name="Today" sheetId="22" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="19" r:id="rId15"/>
+    <sheet name="160818" sheetId="22" r:id="rId14"/>
+    <sheet name="Today" sheetId="23" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'010818'!$C$1:$C$10</definedName>
@@ -34,7 +35,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'100818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'130818'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'140818'!$C$1:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Today!$C$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'160818'!$C$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Today!$C$1:$C$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="197">
   <si>
     <t>#</t>
   </si>
@@ -926,12 +928,30 @@
   <si>
     <t>Gst Mstr_1 to 4</t>
   </si>
+  <si>
+    <t>Worked on HTML report &amp; Gst Mstr_1 to 2</t>
+  </si>
+  <si>
+    <t>Gst Mstr_2 to 6</t>
+  </si>
+  <si>
+    <t>TRA_8 : Transporter can update movement-Completed</t>
+  </si>
+  <si>
+    <t>3.Slow down the scenarios for demo. - Completed</t>
+  </si>
+  <si>
+    <t>Reject scenario</t>
+  </si>
+  <si>
+    <t>All EWB CP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,6 +978,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1147,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1286,6 +1313,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1309,6 +1339,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,7 +1652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1769,36 +1806,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="35" t="s">
         <v>9</v>
       </c>
@@ -1950,36 +1987,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="36" t="s">
         <v>9</v>
       </c>
@@ -2131,36 +2168,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="37" t="s">
         <v>9</v>
       </c>
@@ -2212,7 +2249,7 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="52" t="s">
         <v>174</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -2238,7 +2275,7 @@
       <c r="F5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="9" t="s">
         <v>175</v>
       </c>
@@ -2309,36 +2346,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2445,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2463,36 +2500,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2597,13 +2634,179 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="44.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="46"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="7">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:F35">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H7:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="8:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H7" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2628,36 +2831,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="16" t="s">
         <v>9</v>
       </c>
@@ -2911,36 +3114,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
@@ -3195,36 +3398,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
@@ -3473,36 +3676,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="18" t="s">
         <v>9</v>
       </c>
@@ -3654,36 +3857,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
@@ -3835,36 +4038,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="23" t="s">
         <v>9</v>
       </c>
@@ -4016,36 +4219,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="27" t="s">
         <v>9</v>
       </c>
@@ -4197,36 +4400,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="26" t="s">
         <v>9</v>
       </c>

</xml_diff>